<commit_message>
Ata0104 e alteração no plano de ação
</commit_message>
<xml_diff>
--- a/documentacao/plano de ação.xlsx
+++ b/documentacao/plano de ação.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romullo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romullo\Documents\GitHub\teste\flow\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3868BE-E37C-40FE-852D-AABAFEA0FF1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07295F3-4928-47CD-86CB-54637BD756E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{DF971EFB-ADE0-4EA6-A635-E3D9370C7829}"/>
+    <workbookView xWindow="2340" yWindow="1425" windowWidth="17040" windowHeight="8925" activeTab="1" xr2:uid="{DF971EFB-ADE0-4EA6-A635-E3D9370C7829}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
-  <si>
-    <t>A fazer</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Prioridade</t>
   </si>
@@ -143,7 +140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +151,14 @@
     <font>
       <sz val="36"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -185,15 +190,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AAFFD0-3613-4E2E-908B-D9B42CD42C76}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="A1:E19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,117 +559,117 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -683,7 +689,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,127 +703,127 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1">
         <v>43928</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1">
+        <v>43928</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3">
-        <v>43928</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1">
         <v>43928</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1">
         <v>43928</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="C9" s="1">
         <v>43928</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -825,8 +831,9 @@
     <mergeCell ref="A1:E3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>